<commit_message>
Updated example spreadsheet for version 1.1.0
</commit_message>
<xml_diff>
--- a/quotebookapp_sheet_template.xlsx
+++ b/quotebookapp_sheet_template.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\cs\QuotebookApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C29A8C-9780-40FD-A06C-0BB18968AB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E85472-FF1F-45A6-AA76-2B43B36FF9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Quotes" sheetId="2" r:id="rId2"/>
+    <sheet name="QOTD" sheetId="3" r:id="rId3"/>
+    <sheet name="Reader" sheetId="4" r:id="rId4"/>
+    <sheet name="AppFlag" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -60,6 +63,42 @@
   </si>
   <si>
     <t>Bob: "Hi, John! I'm being quoted!" // Joe: "Cool, that double slash with spaces on either side indicates a new line in this quote!"</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Friendly Name</t>
+  </si>
+  <si>
+    <t>File ID</t>
+  </si>
+  <si>
+    <t>File Size (Bytes)</t>
+  </si>
+  <si>
+    <t>The File ID is the last string of characters in the URL for your Google Drive File. For example, in the URL https://docs.google.com/spreadsheets/d/1qpyC0XzvTcKT6EISywvqESX3A0MwQoFDE8p-Bll4hps/edit#gid=0, the File ID is 1qpyC0XzvTcKT6EISywvqESX3A0MwQoFDE8p-Bll4hps. You can extract the File ID from your Google Drive files in the same way.</t>
+  </si>
+  <si>
+    <t>my_pdf_file</t>
+  </si>
+  <si>
+    <t>My PDF File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Cell A1, put a Y to disable access to the app. Whenever there is a Y there, users will not be able to log in. </t>
+  </si>
+  <si>
+    <t>User Type (A = Admin, N = Normal, I = Invisible)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -70,7 +109,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-m\-d\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -81,6 +120,27 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -110,12 +170,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,13 +398,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -350,8 +419,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -361,8 +433,11 @@
       <c r="C2" s="2">
         <v>1234</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -372,8 +447,11 @@
       <c r="C3" s="2">
         <v>2345</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -383,20 +461,23 @@
       <c r="C4" s="2">
         <v>3456</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
     </row>
   </sheetData>
@@ -411,7 +492,7 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -597,4 +678,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FA440D-DCDF-4188-8CEF-2C4D7F4CAAE8}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A978857-64C1-4075-8244-D87FC7D58194}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>50000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E10894A-9184-4DF2-BBFD-C143319C691D}">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>